<commit_message>
added new care sheets and styles
</commit_message>
<xml_diff>
--- a/data/Reptile Care Sheet.xlsx
+++ b/data/Reptile Care Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hunter\Desktop\Excel\Website\reptilecare\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C38BB39E-D449-4DB2-88A2-FEDF4F7E76AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78C61BBF-73FC-46CD-9287-114047A8A57A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FF7ADF97-DB7D-4853-AEFB-BF2A277B965D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Common Name</t>
   </si>
@@ -61,6 +61,24 @@
   </si>
   <si>
     <t>Crotaphytus collaris</t>
+  </si>
+  <si>
+    <t>Bearded Dragon</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn3.gstatic.com/images?q=tbn:ANd9GcQnrDrTUTwYtSAJEYhsdLHYYsdF2RCjaViWIAeYtIHXXFRQupcs</t>
+  </si>
+  <si>
+    <t>Pogona vitticeps</t>
+  </si>
+  <si>
+    <t>Crested Gecko</t>
+  </si>
+  <si>
+    <t>Correlophus ciliatus</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/d/d9/Crested_gecko_-_1.jpg/800px-Crested_gecko_-_1.jpg</t>
   </si>
 </sst>
 </file>
@@ -428,17 +446,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFB4D42F-A77C-4682-871F-0CECCC46CE04}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="82.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="108.5703125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -474,12 +492,36 @@
         <v>6</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{28052AD4-A0AC-47E7-B952-7664A359A848}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{8BE88066-9C2C-4A09-A865-D7D7077DA158}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{FA0C97C1-1D09-447E-B8E1-46126B4B4301}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{F297AE96-DF1A-4017-9CD2-10242EA14C6F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
change json and readme
</commit_message>
<xml_diff>
--- a/data/Reptile Care Sheet.xlsx
+++ b/data/Reptile Care Sheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mytelespecialists-my.sharepoint.com/personal/hunter_brown_tstelemed_com/Documents/Documents/Website/reptilecare/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{87DA8288-3C59-4C6A-ACA2-1AD87544712A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8744D880-20AE-4A78-B89E-CD907C187498}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{87DA8288-3C59-4C6A-ACA2-1AD87544712A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9F42A562-B38A-4D9E-AD10-4E7C0A52917D}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FF7ADF97-DB7D-4853-AEFB-BF2A277B965D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Common Name</t>
   </si>
@@ -75,19 +75,10 @@
     <t>https://www.karineaigner.com/img-get2/I0000FYAYK6hQ3dQ/sec=/fit=1200x1200/I0000FYAYK6hQ3dQ.jpg</t>
   </si>
   <si>
-    <t>https://i.ibb.co/d0QrLzM/eae731f0-8361-45e6-8912-5c1595285350-1.webp</t>
-  </si>
-  <si>
     <t>https://i.ibb.co/72pZwG7/49108e37e47615b25b854e7978403825-1.jpg</t>
   </si>
   <si>
-    <t>Alignment</t>
-  </si>
-  <si>
-    <t>Left Top</t>
-  </si>
-  <si>
-    <t>Right Top</t>
+    <t>https://geckoadvice.com/wp-content/uploads/2022/03/Leopard-Gecko-Climbing.jpg</t>
   </si>
 </sst>
 </file>
@@ -158,10 +149,14 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -199,7 +194,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -305,7 +300,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -447,7 +442,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -455,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFB4D42F-A77C-4682-871F-0CECCC46CE04}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,10 +461,9 @@
     <col min="1" max="1" width="21.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="97.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -479,11 +473,8 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>15</v>
-      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -491,13 +482,10 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -505,13 +493,10 @@
         <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -521,11 +506,8 @@
       <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>17</v>
-      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -535,15 +517,9 @@
       <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>17</v>
-      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{8C28E6E3-2FD9-4A64-B9C5-E0F54CA339F1}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Remove and replace image
</commit_message>
<xml_diff>
--- a/data/Reptile Care Sheet.xlsx
+++ b/data/Reptile Care Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mytelespecialists-my.sharepoint.com/personal/hunter_brown_tstelemed_com/Documents/Documents/Website/reptilecare/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="13_ncr:1_{87DA8288-3C59-4C6A-ACA2-1AD87544712A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90DF0753-9AB9-4329-8686-6BB95F5604DB}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{87DA8288-3C59-4C6A-ACA2-1AD87544712A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B8361F7A-7474-4A74-A408-E614A9F5C311}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FF7ADF97-DB7D-4853-AEFB-BF2A277B965D}"/>
   </bookViews>
@@ -78,7 +78,7 @@
     <t>https://i.ibb.co/72pZwG7/49108e37e47615b25b854e7978403825-1.jpg</t>
   </si>
   <si>
-    <t>https://geckoadvice.com/wp-content/uploads/2022/03/Leopard-Gecko-Climbing.jpg</t>
+    <t>https://www.robersonreptiles.com/cdn/shop/products/image_f2f0322f-40e6-4df0-857a-4cadd6398fb2_800x.png?v=1669348653</t>
   </si>
 </sst>
 </file>
@@ -449,14 +449,14 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="97.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="116.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
change some image locations
</commit_message>
<xml_diff>
--- a/data/Reptile Care Sheet.xlsx
+++ b/data/Reptile Care Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mytelespecialists-my.sharepoint.com/personal/hunter_brown_tstelemed_com/Documents/Documents/Website/reptilecare/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="82" documentId="13_ncr:1_{87DA8288-3C59-4C6A-ACA2-1AD87544712A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A3818E0F-76BA-4D0D-80CB-DEEB63DB7ACE}"/>
+  <xr:revisionPtr revIDLastSave="85" documentId="13_ncr:1_{87DA8288-3C59-4C6A-ACA2-1AD87544712A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE36C0E7-1F65-4D24-B722-8A30FC751ACA}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FF7ADF97-DB7D-4853-AEFB-BF2A277B965D}"/>
+    <workbookView minimized="1" xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11295" xr2:uid="{FF7ADF97-DB7D-4853-AEFB-BF2A277B965D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -539,7 +539,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -669,7 +669,12 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:H5" xr:uid="{BFB4D42F-A77C-4682-871F-0CECCC46CE04}"/>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{8B22D278-D0C0-4167-B09A-AEB5E3B7FDF5}"/>
+    <hyperlink ref="E4" r:id="rId2" xr:uid="{27A4F056-A464-45A5-BE09-09C88746BEBD}"/>
+    <hyperlink ref="E3" r:id="rId3" xr:uid="{FFD3A402-7229-4577-AADE-4B07980881FB}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>